<commit_message>
when user tries to save TPA or TTT which already exists in DB. The manifest with such TPA or TTT should have status isActive = false.
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
+++ b/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
@@ -1347,21 +1347,7 @@
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -1814,9 +1800,9 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,7 +1947,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="47" t="n">
-        <v>43919.0</v>
+        <v>43922.0</v>
       </c>
       <c r="C3" s="58" t="n">
         <v>0.4375</v>
@@ -1973,7 +1959,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="38" t="n">
-        <v>43920.0</v>
+        <v>43923.0</v>
       </c>
       <c r="G3" s="40" t="n">
         <v>0.6458333333333334</v>
@@ -1989,7 +1975,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="44" t="n">
-        <v>43922.0</v>
+        <v>43925.0</v>
       </c>
       <c r="O3" s="49" t="n">
         <v>0.4583333333333333</v>
@@ -2001,7 +1987,7 @@
         <v>136</v>
       </c>
       <c r="R3" s="45" t="n">
-        <v>43935.0</v>
+        <v>43938.0</v>
       </c>
       <c r="S3" s="69" t="n">
         <v>0.4166666666666667</v>
@@ -2030,7 +2016,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="37" t="n">
-        <v>43918.0</v>
+        <v>43921.0</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>0.4791666666666667</v>
@@ -2042,7 +2028,7 @@
         <v>113</v>
       </c>
       <c r="F4" s="39" t="n">
-        <v>43918.0</v>
+        <v>43921.0</v>
       </c>
       <c r="G4" s="40" t="n">
         <v>0.6875</v>
@@ -2054,7 +2040,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="42" t="n">
-        <v>43921.0</v>
+        <v>43924.0</v>
       </c>
       <c r="K4" s="51" t="n">
         <v>0.5277777777777778</v>
@@ -2066,7 +2052,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="41" t="n">
-        <v>43923.0</v>
+        <v>43926.0</v>
       </c>
       <c r="O4" s="48" t="n">
         <v>0.7083333333333334</v>
@@ -2078,7 +2064,7 @@
         <v>137</v>
       </c>
       <c r="R4" s="46" t="n">
-        <v>43927.0</v>
+        <v>43930.0</v>
       </c>
       <c r="S4" s="71" t="n">
         <v>0.5</v>
@@ -2104,7 +2090,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="37" t="n">
-        <v>43914.0</v>
+        <v>43917.0</v>
       </c>
       <c r="C5" s="56" t="n">
         <v>0.3541666666666667</v>
@@ -2116,7 +2102,7 @@
         <v>115</v>
       </c>
       <c r="F5" s="38" t="n">
-        <v>43917.0</v>
+        <v>43920.0</v>
       </c>
       <c r="G5" s="40" t="n">
         <v>0.4375</v>
@@ -2128,7 +2114,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="42" t="n">
-        <v>43920.0</v>
+        <v>43923.0</v>
       </c>
       <c r="K5" s="51" t="n">
         <v>0.5798611111111112</v>
@@ -2140,7 +2126,7 @@
         <v>111</v>
       </c>
       <c r="N5" s="44">
-        <v>43922</v>
+        <v>43924</v>
       </c>
       <c r="O5" s="49">
         <v>0.375</v>
@@ -2152,7 +2138,7 @@
         <v>134</v>
       </c>
       <c r="R5" s="46" t="n">
-        <v>43921.0</v>
+        <v>43924.0</v>
       </c>
       <c r="S5" s="71" t="n">
         <v>0.7083333333333334</v>
@@ -2183,68 +2169,68 @@
     <mergeCell ref="I1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:L2994">
-    <cfRule type="expression" dxfId="25" priority="23">
+    <cfRule type="expression" dxfId="23" priority="23">
       <formula>OR(NOT(VLOOKUP($H3,$H:$K,4,0)=$K3),NOT(VLOOKUP($H3,$H:$J,3,0)=$J3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:O4 L6:O2994 L5">
-    <cfRule type="expression" dxfId="24" priority="22">
+    <cfRule type="expression" dxfId="22" priority="22">
       <formula>OR(NOT(VLOOKUP($L3,$L:$O,4,0)=$O3),NOT(VLOOKUP($L3,$L:$N,3,0)=$N3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:D2994">
-    <cfRule type="expression" dxfId="23" priority="34">
+    <cfRule type="expression" dxfId="21" priority="34">
       <formula>AND(OR(ISBLANK($B3),ISBLANK($C3),NOT(TYPE($B3)=1),NOT(TYPE($C3)=1)),NOT(ISBLANK($A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G2994">
-    <cfRule type="expression" dxfId="22" priority="17">
+    <cfRule type="expression" dxfId="20" priority="17">
       <formula>AND(OR(ISBLANK($F3),ISBLANK($G3),NOT(TYPE($F3)=1),NOT(TYPE($G3)=1)),NOT(ISBLANK($E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K2994">
-    <cfRule type="expression" dxfId="21" priority="16">
+    <cfRule type="expression" dxfId="19" priority="16">
       <formula>AND(OR(ISBLANK($J3),ISBLANK($K3),NOT(TYPE($J3)=1),NOT(TYPE($K3)=1)),NOT(ISBLANK($I3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:O4 N6:O2994">
-    <cfRule type="expression" dxfId="20" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>AND(OR(ISBLANK($N3),ISBLANK($O3),NOT(TYPE($N3)=1),NOT(TYPE($O3)=1)),NOT(ISBLANK($M3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:S2994">
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>AND(OR(ISBLANK($R3),ISBLANK($S3),NOT(TYPE($R3)=1),NOT(TYPE($S3)=1)),NOT(ISBLANK($Q3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D3000">
-    <cfRule type="expression" dxfId="19" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>NOT(AND(B3=INDEX($B$3:$B$3000,MATCH(D3,$D$3:$D$3000,0)),C3=INDEX($C$3:$C$3000,MATCH(D3,$D$3:$D$3000,0))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>AND(NOT(ISBLANK($A3)),ISBLANK($D3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T3382">
-    <cfRule type="duplicateValues" dxfId="17" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5 O5">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>OR(NOT(VLOOKUP($L5,$L:$O,4,0)=$O5),NOT(VLOOKUP($L5,$L:$N,3,0)=$N5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>AND(OR(ISBLANK($N5),ISBLANK($O5),NOT(TYPE($N5)=1),NOT(TYPE($O5)=1)),NOT(ISBLANK($M5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>OR(NOT(VLOOKUP($L5,$L:$O,4,0)=$O5),NOT(VLOOKUP($L5,$L:$N,3,0)=$N5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>AND(OR(ISBLANK($N5),ISBLANK($O5),NOT(TYPE($N5)=1),NOT(TYPE($O5)=1)),NOT(ISBLANK($M5)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Test case if there No Wh-Customer settings in DB for pare Customer Warehouse.
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
+++ b/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
@@ -1947,7 +1947,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="47" t="n">
-        <v>43922.0</v>
+        <v>43933.0</v>
       </c>
       <c r="C3" s="58" t="n">
         <v>0.4375</v>
@@ -1959,7 +1959,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="38" t="n">
-        <v>43923.0</v>
+        <v>43934.0</v>
       </c>
       <c r="G3" s="40" t="n">
         <v>0.6458333333333334</v>
@@ -1975,7 +1975,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="44" t="n">
-        <v>43925.0</v>
+        <v>43936.0</v>
       </c>
       <c r="O3" s="49" t="n">
         <v>0.4583333333333333</v>
@@ -1987,7 +1987,7 @@
         <v>136</v>
       </c>
       <c r="R3" s="45" t="n">
-        <v>43938.0</v>
+        <v>43949.0</v>
       </c>
       <c r="S3" s="69" t="n">
         <v>0.4166666666666667</v>
@@ -2016,7 +2016,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="37" t="n">
-        <v>43921.0</v>
+        <v>43932.0</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>0.4791666666666667</v>
@@ -2028,7 +2028,7 @@
         <v>113</v>
       </c>
       <c r="F4" s="39" t="n">
-        <v>43921.0</v>
+        <v>43932.0</v>
       </c>
       <c r="G4" s="40" t="n">
         <v>0.6875</v>
@@ -2040,7 +2040,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="42" t="n">
-        <v>43924.0</v>
+        <v>43935.0</v>
       </c>
       <c r="K4" s="51" t="n">
         <v>0.5277777777777778</v>
@@ -2052,7 +2052,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="41" t="n">
-        <v>43926.0</v>
+        <v>43937.0</v>
       </c>
       <c r="O4" s="48" t="n">
         <v>0.7083333333333334</v>
@@ -2064,7 +2064,7 @@
         <v>137</v>
       </c>
       <c r="R4" s="46" t="n">
-        <v>43930.0</v>
+        <v>43941.0</v>
       </c>
       <c r="S4" s="71" t="n">
         <v>0.5</v>
@@ -2090,7 +2090,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="37" t="n">
-        <v>43917.0</v>
+        <v>43928.0</v>
       </c>
       <c r="C5" s="56" t="n">
         <v>0.3541666666666667</v>
@@ -2102,7 +2102,7 @@
         <v>115</v>
       </c>
       <c r="F5" s="38" t="n">
-        <v>43920.0</v>
+        <v>43931.0</v>
       </c>
       <c r="G5" s="40" t="n">
         <v>0.4375</v>
@@ -2114,7 +2114,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="42" t="n">
-        <v>43923.0</v>
+        <v>43933.0</v>
       </c>
       <c r="K5" s="51" t="n">
         <v>0.5798611111111112</v>
@@ -2125,10 +2125,10 @@
       <c r="M5" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N5" s="44">
-        <v>43924</v>
+      <c r="N5" s="44" t="n">
+        <v>43935.0</v>
       </c>
-      <c r="O5" s="49">
+      <c r="O5" s="49" t="n">
         <v>0.375</v>
       </c>
       <c r="P5" s="10" t="s">
@@ -2138,7 +2138,7 @@
         <v>134</v>
       </c>
       <c r="R5" s="46" t="n">
-        <v>43924.0</v>
+        <v>43936.0</v>
       </c>
       <c r="S5" s="71" t="n">
         <v>0.7083333333333334</v>

</xml_diff>

<commit_message>
ExcelManifestValidator created as validator of entities from POST requests from ExcelManifestController. Validation Methods were moved from ExcelManifestController to ExcelManifestValidator. Save method and methods of connection TPA, TTT, ManifestReference and Manifest from ExcelManifestController moved to TruckService.
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
+++ b/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
@@ -1947,7 +1947,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="47" t="n">
-        <v>43933.0</v>
+        <v>43936.0</v>
       </c>
       <c r="C3" s="58" t="n">
         <v>0.4375</v>
@@ -1959,7 +1959,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="38" t="n">
-        <v>43934.0</v>
+        <v>43937.0</v>
       </c>
       <c r="G3" s="40" t="n">
         <v>0.6458333333333334</v>
@@ -1975,7 +1975,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="44" t="n">
-        <v>43936.0</v>
+        <v>43939.0</v>
       </c>
       <c r="O3" s="49" t="n">
         <v>0.4583333333333333</v>
@@ -1987,7 +1987,7 @@
         <v>136</v>
       </c>
       <c r="R3" s="45" t="n">
-        <v>43949.0</v>
+        <v>43952.0</v>
       </c>
       <c r="S3" s="69" t="n">
         <v>0.4166666666666667</v>
@@ -2016,7 +2016,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="37" t="n">
-        <v>43932.0</v>
+        <v>43935.0</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>0.4791666666666667</v>
@@ -2028,7 +2028,7 @@
         <v>113</v>
       </c>
       <c r="F4" s="39" t="n">
-        <v>43932.0</v>
+        <v>43935.0</v>
       </c>
       <c r="G4" s="40" t="n">
         <v>0.6875</v>
@@ -2040,7 +2040,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="42" t="n">
-        <v>43935.0</v>
+        <v>43938.0</v>
       </c>
       <c r="K4" s="51" t="n">
         <v>0.5277777777777778</v>
@@ -2052,7 +2052,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="41" t="n">
-        <v>43937.0</v>
+        <v>43940.0</v>
       </c>
       <c r="O4" s="48" t="n">
         <v>0.7083333333333334</v>
@@ -2064,7 +2064,7 @@
         <v>137</v>
       </c>
       <c r="R4" s="46" t="n">
-        <v>43941.0</v>
+        <v>43944.0</v>
       </c>
       <c r="S4" s="71" t="n">
         <v>0.5</v>
@@ -2090,7 +2090,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="37" t="n">
-        <v>43928.0</v>
+        <v>43931.0</v>
       </c>
       <c r="C5" s="56" t="n">
         <v>0.3541666666666667</v>
@@ -2102,7 +2102,7 @@
         <v>115</v>
       </c>
       <c r="F5" s="38" t="n">
-        <v>43931.0</v>
+        <v>43934.0</v>
       </c>
       <c r="G5" s="40" t="n">
         <v>0.4375</v>
@@ -2114,7 +2114,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="42" t="n">
-        <v>43933.0</v>
+        <v>43936.0</v>
       </c>
       <c r="K5" s="51" t="n">
         <v>0.5798611111111112</v>
@@ -2126,7 +2126,7 @@
         <v>111</v>
       </c>
       <c r="N5" s="44" t="n">
-        <v>43935.0</v>
+        <v>43938.0</v>
       </c>
       <c r="O5" s="49" t="n">
         <v>0.375</v>
@@ -2138,7 +2138,7 @@
         <v>134</v>
       </c>
       <c r="R5" s="46" t="n">
-        <v>43936.0</v>
+        <v>43939.0</v>
       </c>
       <c r="S5" s="71" t="n">
         <v>0.7083333333333334</v>

</xml_diff>

<commit_message>
backup commit of files after system crash
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
+++ b/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
@@ -1947,7 +1947,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="47" t="n">
-        <v>43936.0</v>
+        <v>43942.0</v>
       </c>
       <c r="C3" s="58" t="n">
         <v>0.4375</v>
@@ -1959,7 +1959,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="38" t="n">
-        <v>43937.0</v>
+        <v>43943.0</v>
       </c>
       <c r="G3" s="40" t="n">
         <v>0.6458333333333334</v>
@@ -1975,7 +1975,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="44" t="n">
-        <v>43939.0</v>
+        <v>43945.0</v>
       </c>
       <c r="O3" s="49" t="n">
         <v>0.4583333333333333</v>
@@ -1987,7 +1987,7 @@
         <v>136</v>
       </c>
       <c r="R3" s="45" t="n">
-        <v>43952.0</v>
+        <v>43958.0</v>
       </c>
       <c r="S3" s="69" t="n">
         <v>0.4166666666666667</v>
@@ -2016,7 +2016,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="37" t="n">
-        <v>43935.0</v>
+        <v>43941.0</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>0.4791666666666667</v>
@@ -2028,7 +2028,7 @@
         <v>113</v>
       </c>
       <c r="F4" s="39" t="n">
-        <v>43935.0</v>
+        <v>43941.0</v>
       </c>
       <c r="G4" s="40" t="n">
         <v>0.6875</v>
@@ -2040,7 +2040,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="42" t="n">
-        <v>43938.0</v>
+        <v>43944.0</v>
       </c>
       <c r="K4" s="51" t="n">
         <v>0.5277777777777778</v>
@@ -2052,7 +2052,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="41" t="n">
-        <v>43940.0</v>
+        <v>43946.0</v>
       </c>
       <c r="O4" s="48" t="n">
         <v>0.7083333333333334</v>
@@ -2064,7 +2064,7 @@
         <v>137</v>
       </c>
       <c r="R4" s="46" t="n">
-        <v>43944.0</v>
+        <v>43950.0</v>
       </c>
       <c r="S4" s="71" t="n">
         <v>0.5</v>
@@ -2090,7 +2090,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="37" t="n">
-        <v>43931.0</v>
+        <v>43937.0</v>
       </c>
       <c r="C5" s="56" t="n">
         <v>0.3541666666666667</v>
@@ -2102,7 +2102,7 @@
         <v>115</v>
       </c>
       <c r="F5" s="38" t="n">
-        <v>43934.0</v>
+        <v>43940.0</v>
       </c>
       <c r="G5" s="40" t="n">
         <v>0.4375</v>
@@ -2114,7 +2114,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="42" t="n">
-        <v>43936.0</v>
+        <v>43942.0</v>
       </c>
       <c r="K5" s="51" t="n">
         <v>0.5798611111111112</v>
@@ -2126,7 +2126,7 @@
         <v>111</v>
       </c>
       <c r="N5" s="44" t="n">
-        <v>43938.0</v>
+        <v>43944.0</v>
       </c>
       <c r="O5" s="49" t="n">
         <v>0.375</v>
@@ -2138,7 +2138,7 @@
         <v>134</v>
       </c>
       <c r="R5" s="46" t="n">
-        <v>43939.0</v>
+        <v>43945.0</v>
       </c>
       <c r="S5" s="71" t="n">
         <v>0.7083333333333334</v>

</xml_diff>

<commit_message>
TPA controller Update action. TPA Update tests. TTT Update Tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
+++ b/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FF6313-DB88-4B54-8EC3-380E38825600}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MANIFESTS" sheetId="4" r:id="rId1"/>
@@ -21,7 +22,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -545,7 +546,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -1796,7 +1797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Z5"/>
   <sheetViews>
@@ -1807,23 +1808,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="7.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="6.85546875" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1946,10 +1947,10 @@
       <c r="A3" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="47" t="n">
-        <v>43942.0</v>
+      <c r="B3" s="47">
+        <v>43972</v>
       </c>
-      <c r="C3" s="58" t="n">
+      <c r="C3" s="58">
         <v>0.4375</v>
       </c>
       <c r="D3" s="58" t="s">
@@ -1958,11 +1959,11 @@
       <c r="E3" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="38" t="n">
-        <v>43943.0</v>
+      <c r="F3" s="38">
+        <v>43973</v>
       </c>
-      <c r="G3" s="40" t="n">
-        <v>0.6458333333333334</v>
+      <c r="G3" s="40">
+        <v>0.64583333333333337</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>139</v>
@@ -1974,11 +1975,11 @@
       <c r="M3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N3" s="44" t="n">
-        <v>43945.0</v>
+      <c r="N3" s="44">
+        <v>43975</v>
       </c>
-      <c r="O3" s="49" t="n">
-        <v>0.4583333333333333</v>
+      <c r="O3" s="49">
+        <v>0.45833333333333331</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>109</v>
@@ -1986,11 +1987,11 @@
       <c r="Q3" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="R3" s="45" t="n">
-        <v>43958.0</v>
+      <c r="R3" s="45">
+        <v>43989</v>
       </c>
-      <c r="S3" s="69" t="n">
-        <v>0.4166666666666667</v>
+      <c r="S3" s="69">
+        <v>0.41666666666666669</v>
       </c>
       <c r="T3" s="32" t="s">
         <v>96</v>
@@ -2015,11 +2016,11 @@
       <c r="A4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="37" t="n">
-        <v>43941.0</v>
+      <c r="B4" s="37">
+        <v>43971</v>
       </c>
-      <c r="C4" s="56" t="n">
-        <v>0.4791666666666667</v>
+      <c r="C4" s="56">
+        <v>0.47916666666666669</v>
       </c>
       <c r="D4" s="56" t="s">
         <v>103</v>
@@ -2027,10 +2028,10 @@
       <c r="E4" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="39" t="n">
-        <v>43941.0</v>
+      <c r="F4" s="39">
+        <v>43971</v>
       </c>
-      <c r="G4" s="40" t="n">
+      <c r="G4" s="40">
         <v>0.6875</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -2039,11 +2040,11 @@
       <c r="I4" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="42" t="n">
-        <v>43944.0</v>
+      <c r="J4" s="42">
+        <v>43974</v>
       </c>
-      <c r="K4" s="51" t="n">
-        <v>0.5277777777777778</v>
+      <c r="K4" s="51">
+        <v>0.52777777777777779</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>105</v>
@@ -2051,11 +2052,11 @@
       <c r="M4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N4" s="41" t="n">
-        <v>43946.0</v>
+      <c r="N4" s="41">
+        <v>43976</v>
       </c>
-      <c r="O4" s="48" t="n">
-        <v>0.7083333333333334</v>
+      <c r="O4" s="48">
+        <v>0.70833333333333337</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>110</v>
@@ -2063,10 +2064,10 @@
       <c r="Q4" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="R4" s="46" t="n">
-        <v>43950.0</v>
+      <c r="R4" s="46">
+        <v>43980</v>
       </c>
-      <c r="S4" s="71" t="n">
+      <c r="S4" s="71">
         <v>0.5</v>
       </c>
       <c r="T4" s="33" t="s">
@@ -2089,11 +2090,11 @@
       <c r="A5" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="37" t="n">
-        <v>43937.0</v>
+      <c r="B5" s="37">
+        <v>43976</v>
       </c>
-      <c r="C5" s="56" t="n">
-        <v>0.3541666666666667</v>
+      <c r="C5" s="56">
+        <v>0.35416666666666669</v>
       </c>
       <c r="D5" s="56" t="s">
         <v>104</v>
@@ -2101,10 +2102,10 @@
       <c r="E5" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="38" t="n">
-        <v>43940.0</v>
+      <c r="F5" s="38">
+        <v>43977</v>
       </c>
-      <c r="G5" s="40" t="n">
+      <c r="G5" s="40">
         <v>0.4375</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -2113,11 +2114,11 @@
       <c r="I5" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="J5" s="42" t="n">
-        <v>43942.0</v>
+      <c r="J5" s="42">
+        <v>43978</v>
       </c>
-      <c r="K5" s="51" t="n">
-        <v>0.5798611111111112</v>
+      <c r="K5" s="51">
+        <v>0.57986111111111116</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>108</v>
@@ -2125,10 +2126,10 @@
       <c r="M5" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N5" s="44" t="n">
-        <v>43944.0</v>
+      <c r="N5" s="44">
+        <v>43980</v>
       </c>
-      <c r="O5" s="49" t="n">
+      <c r="O5" s="49">
         <v>0.375</v>
       </c>
       <c r="P5" s="10" t="s">
@@ -2137,11 +2138,11 @@
       <c r="Q5" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="R5" s="46" t="n">
-        <v>43945.0</v>
+      <c r="R5" s="46">
+        <v>43986</v>
       </c>
-      <c r="S5" s="71" t="n">
-        <v>0.7083333333333334</v>
+      <c r="S5" s="71">
+        <v>0.70833333333333337</v>
       </c>
       <c r="T5" s="33" t="s">
         <v>98</v>
@@ -2344,7 +2345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -2355,13 +2356,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2451,7 +2452,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D2"/>
+  <autoFilter ref="A2:D2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
@@ -2462,7 +2463,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="2" id="{2422F177-28FB-44CF-A4DE-B7E2DAB6F9D1}">
@@ -2497,7 +2498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:I1247"/>
   <sheetViews>
@@ -2508,12 +2509,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="13.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -16360,7 +16361,7 @@
       <c r="I1247" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H2"/>
+  <autoFilter ref="A2:H2" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="9">
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:G2"/>
@@ -16377,7 +16378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Лист4"/>
   <dimension ref="A1:J1387"/>
   <sheetViews>
@@ -16388,13 +16389,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="13.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -33162,7 +33163,7 @@
       <c r="J1387" s="62"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H2"/>
+  <autoFilter ref="A2:H2" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="10">
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
@@ -33180,9 +33181,9 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Лист5"/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
@@ -33190,8 +33191,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="6" width="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33406,11 +33407,11 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
ManifestController addReference to Manifest reviewed
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
+++ b/src/test/resources/excelTests/manifestREferenceSupplCustCompareToRefereneceSupplCust.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FF6313-DB88-4B54-8EC3-380E38825600}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61670258-D9D2-40A6-8A4B-B682A41ABBC5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -46,7 +46,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>Автор:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -1117,7 +1117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1343,10 +1343,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1803,7 +1804,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="4" sqref="R3:R5 N3:N5 J4:J5 F3:F5 B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1949,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="47">
-        <v>43972</v>
+        <v>44104</v>
       </c>
       <c r="C3" s="58">
         <v>0.4375</v>
@@ -1960,7 +1961,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="38">
-        <v>43973</v>
+        <v>44105</v>
       </c>
       <c r="G3" s="40">
         <v>0.64583333333333337</v>
@@ -1976,7 +1977,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="44">
-        <v>43975</v>
+        <v>44107</v>
       </c>
       <c r="O3" s="49">
         <v>0.45833333333333331</v>
@@ -1988,7 +1989,7 @@
         <v>136</v>
       </c>
       <c r="R3" s="45">
-        <v>43989</v>
+        <v>44121</v>
       </c>
       <c r="S3" s="69">
         <v>0.41666666666666669</v>
@@ -2017,7 +2018,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="37">
-        <v>43971</v>
+        <v>44103</v>
       </c>
       <c r="C4" s="56">
         <v>0.47916666666666669</v>
@@ -2029,7 +2030,7 @@
         <v>113</v>
       </c>
       <c r="F4" s="39">
-        <v>43971</v>
+        <v>44103</v>
       </c>
       <c r="G4" s="40">
         <v>0.6875</v>
@@ -2041,7 +2042,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="42">
-        <v>43974</v>
+        <v>44106</v>
       </c>
       <c r="K4" s="51">
         <v>0.52777777777777779</v>
@@ -2053,7 +2054,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="41">
-        <v>43976</v>
+        <v>44108</v>
       </c>
       <c r="O4" s="48">
         <v>0.70833333333333337</v>
@@ -2065,7 +2066,7 @@
         <v>137</v>
       </c>
       <c r="R4" s="46">
-        <v>43980</v>
+        <v>44112</v>
       </c>
       <c r="S4" s="71">
         <v>0.5</v>
@@ -2085,13 +2086,16 @@
       <c r="X4" s="16">
         <v>2.4</v>
       </c>
+      <c r="Z4" s="103">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="37">
-        <v>43976</v>
+        <v>44108</v>
       </c>
       <c r="C5" s="56">
         <v>0.35416666666666669</v>
@@ -2103,7 +2107,7 @@
         <v>115</v>
       </c>
       <c r="F5" s="38">
-        <v>43977</v>
+        <v>44109</v>
       </c>
       <c r="G5" s="40">
         <v>0.4375</v>
@@ -2115,7 +2119,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="42">
-        <v>43978</v>
+        <v>44110</v>
       </c>
       <c r="K5" s="51">
         <v>0.57986111111111116</v>
@@ -2127,7 +2131,7 @@
         <v>111</v>
       </c>
       <c r="N5" s="44">
-        <v>43980</v>
+        <v>44112</v>
       </c>
       <c r="O5" s="49">
         <v>0.375</v>
@@ -2139,7 +2143,7 @@
         <v>134</v>
       </c>
       <c r="R5" s="46">
-        <v>43986</v>
+        <v>44118</v>
       </c>
       <c r="S5" s="71">
         <v>0.70833333333333337</v>

</xml_diff>